<commit_message>
feat: Implemented county column functionality and updated data file
</commit_message>
<xml_diff>
--- a/Failure_DB_List_2_updated.xlsx
+++ b/Failure_DB_List_2_updated.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\QT 2025\BESS Failure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6B8561-F8BA-48D8-AA02-37A973EB9EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5219B3-905B-4229-9D40-1A4DC8A69908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{798CB373-87E7-49EA-BBB3-39A2A4BDAAA9}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="676">
   <si>
     <t>Location</t>
   </si>
@@ -2029,6 +2029,51 @@
   </si>
   <si>
     <t>https://www.pressandjournal.co.uk/battery-fire-rothienorman-incident-report</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Usa</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Canada</t>
   </si>
 </sst>
 </file>
@@ -2875,13 +2920,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497C55DF-93CF-4D1D-A370-8C68827540EC}">
-  <dimension ref="A1:Z95"/>
+  <dimension ref="A1:AA95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Y75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U2" sqref="U2:U94"/>
+      <selection pane="bottomRight" activeCell="AA96" sqref="AA96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2908,9 +2953,10 @@
     <col min="23" max="23" width="104.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="169.109375" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2989,8 +3035,11 @@
       <c r="Z1" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -3028,8 +3077,11 @@
       <c r="V2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA2" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3078,8 +3130,11 @@
       <c r="W3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA3" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -3113,8 +3168,11 @@
       <c r="V4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA4" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -3143,8 +3201,11 @@
       <c r="U5" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA5" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -3178,8 +3239,11 @@
       <c r="V6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA6" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -3202,8 +3266,11 @@
       <c r="U7" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA7" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -3237,8 +3304,11 @@
       <c r="U8" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA8" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -3276,8 +3346,11 @@
       <c r="W9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA9" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -3300,8 +3373,11 @@
       <c r="U10" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA10" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>78</v>
       </c>
@@ -3341,8 +3417,11 @@
       <c r="U11" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA11" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -3385,8 +3464,11 @@
       <c r="U12" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA12" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -3435,8 +3517,11 @@
       <c r="U13" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA13" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -3479,8 +3564,11 @@
       <c r="U14" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA14" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -3523,8 +3611,11 @@
       <c r="U15" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA15" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -3567,8 +3658,11 @@
       <c r="U16" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA16" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>105</v>
       </c>
@@ -3611,8 +3705,11 @@
       <c r="U17" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA17" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -3655,8 +3752,11 @@
       <c r="U18" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA18" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -3702,8 +3802,11 @@
       <c r="U19" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA19" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -3752,8 +3855,11 @@
       <c r="U20" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA20" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>125</v>
       </c>
@@ -3796,8 +3902,11 @@
       <c r="U21" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA21" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -3843,8 +3952,11 @@
       <c r="U22" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA22" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -3884,8 +3996,11 @@
       <c r="U23" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA23" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -3925,8 +4040,11 @@
       <c r="U24" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA24" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -3966,8 +4084,11 @@
       <c r="U25" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA25" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -4004,8 +4125,11 @@
       <c r="U26" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA26" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>135</v>
       </c>
@@ -4048,8 +4172,11 @@
       <c r="U27" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA27" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>138</v>
       </c>
@@ -4095,8 +4222,11 @@
       <c r="U28" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA28" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>142</v>
       </c>
@@ -4130,8 +4260,11 @@
       <c r="U29" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA29" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -4165,8 +4298,11 @@
       <c r="U30" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA30" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -4200,8 +4336,11 @@
       <c r="U31" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA31" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>150</v>
       </c>
@@ -4256,8 +4395,11 @@
       <c r="U32" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA32" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>161</v>
       </c>
@@ -4300,8 +4442,11 @@
       <c r="U33" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA33" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>142</v>
       </c>
@@ -4341,8 +4486,11 @@
       <c r="U34" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AA34" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -4388,8 +4536,11 @@
       <c r="U35" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA35" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>171</v>
       </c>
@@ -4418,8 +4569,11 @@
       <c r="U36" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA36" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>176</v>
       </c>
@@ -4462,8 +4616,11 @@
       <c r="U37" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AA37" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>178</v>
       </c>
@@ -4509,8 +4666,11 @@
       <c r="U38" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AA38" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>181</v>
       </c>
@@ -4556,8 +4716,11 @@
       <c r="U39" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AA39" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>184</v>
       </c>
@@ -4597,8 +4760,11 @@
       <c r="U40" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA40" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>186</v>
       </c>
@@ -4626,8 +4792,11 @@
       <c r="U41" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA41" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>190</v>
       </c>
@@ -4673,8 +4842,11 @@
       <c r="U42" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA42" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>196</v>
       </c>
@@ -4726,8 +4898,11 @@
       <c r="U43" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA43" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>202</v>
       </c>
@@ -4779,8 +4954,11 @@
       <c r="U44" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA44" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>210</v>
       </c>
@@ -4809,8 +4987,11 @@
       <c r="U45" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA45" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>214</v>
       </c>
@@ -4836,8 +5017,11 @@
       <c r="U46" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA46" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>216</v>
       </c>
@@ -4871,8 +5055,11 @@
       <c r="U47" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AA47" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>219</v>
       </c>
@@ -4918,8 +5105,11 @@
       <c r="U48" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA48" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>227</v>
       </c>
@@ -4971,8 +5161,11 @@
       <c r="W49" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA49" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>236</v>
       </c>
@@ -5004,8 +5197,11 @@
       <c r="U50" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA50" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>239</v>
       </c>
@@ -5034,8 +5230,11 @@
       <c r="U51" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA51" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>244</v>
       </c>
@@ -5084,8 +5283,11 @@
       <c r="W52" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA52" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>254</v>
       </c>
@@ -5137,8 +5339,11 @@
       <c r="U53" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA53" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>261</v>
       </c>
@@ -5205,8 +5410,11 @@
       <c r="W54" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA54" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>270</v>
       </c>
@@ -5261,8 +5469,11 @@
       <c r="W55" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA55" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>279</v>
       </c>
@@ -5311,8 +5522,11 @@
       <c r="U56" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA56" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>289</v>
       </c>
@@ -5358,8 +5572,11 @@
       <c r="U57" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA57" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>270</v>
       </c>
@@ -5420,8 +5637,11 @@
       <c r="W58" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA58" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>297</v>
       </c>
@@ -5464,8 +5684,11 @@
       <c r="U59" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA59" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>300</v>
       </c>
@@ -5517,8 +5740,11 @@
       <c r="U60" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA60" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>306</v>
       </c>
@@ -5561,8 +5787,11 @@
       <c r="U61" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA61" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>309</v>
       </c>
@@ -5588,8 +5817,11 @@
       <c r="U62" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA62" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>311</v>
       </c>
@@ -5632,8 +5864,11 @@
       <c r="U63" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA63" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>318</v>
       </c>
@@ -5668,8 +5903,11 @@
       <c r="U64" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA64" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>321</v>
       </c>
@@ -5698,8 +5936,11 @@
       <c r="U65" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="66" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA65" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>270</v>
       </c>
@@ -5760,8 +6001,11 @@
       <c r="W66" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA66" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>331</v>
       </c>
@@ -5804,8 +6048,11 @@
       <c r="U67" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA67" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>336</v>
       </c>
@@ -5848,8 +6095,11 @@
       <c r="U68" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA68" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>339</v>
       </c>
@@ -5889,8 +6139,11 @@
       <c r="U69" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA69" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>342</v>
       </c>
@@ -5931,8 +6184,11 @@
       <c r="U70" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA70" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>349</v>
       </c>
@@ -5958,8 +6214,11 @@
       <c r="U71" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA71" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>354</v>
       </c>
@@ -6008,8 +6267,11 @@
       <c r="U72" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA72" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>360</v>
       </c>
@@ -6058,8 +6320,11 @@
       <c r="U73" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA73" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>366</v>
       </c>
@@ -6120,8 +6385,11 @@
       <c r="U74" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="75" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA74" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>366</v>
       </c>
@@ -6182,8 +6450,11 @@
       <c r="U75" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA75" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>297</v>
       </c>
@@ -6218,8 +6489,11 @@
       <c r="U76" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA76" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>383</v>
       </c>
@@ -6277,8 +6551,11 @@
       <c r="U77" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA77" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>389</v>
       </c>
@@ -6304,8 +6581,11 @@
       <c r="U78" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA78" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>393</v>
       </c>
@@ -6351,8 +6631,11 @@
       <c r="U79" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AA79" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>300</v>
       </c>
@@ -6401,8 +6684,11 @@
       <c r="U80" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA80" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>402</v>
       </c>
@@ -6454,8 +6740,11 @@
       <c r="U81" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA81" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>405</v>
       </c>
@@ -6493,8 +6782,11 @@
       <c r="U82" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA82" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>410</v>
       </c>
@@ -6552,8 +6844,11 @@
       <c r="U83" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="84" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA83" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>416</v>
       </c>
@@ -6585,8 +6880,11 @@
       <c r="U84" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA84" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>418</v>
       </c>
@@ -6629,8 +6927,11 @@
       <c r="U85" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA85" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>424</v>
       </c>
@@ -6653,8 +6954,11 @@
       <c r="U86" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA86" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>427</v>
       </c>
@@ -6677,8 +6981,11 @@
       <c r="U87" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA87" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>430</v>
       </c>
@@ -6721,8 +7028,11 @@
       <c r="U88" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA88" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>436</v>
       </c>
@@ -6754,8 +7064,11 @@
       <c r="U89" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA89" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>442</v>
       </c>
@@ -6787,8 +7100,11 @@
       <c r="U90" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="91" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AA90" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>270</v>
       </c>
@@ -6843,8 +7159,11 @@
       <c r="W91" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA91" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>452</v>
       </c>
@@ -6884,8 +7203,11 @@
       <c r="U92" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA92" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>459</v>
       </c>
@@ -6928,8 +7250,11 @@
       <c r="U93" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA93" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>463</v>
       </c>
@@ -6981,8 +7306,11 @@
       <c r="W94" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA94" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>472</v>
       </c>
@@ -7006,6 +7334,9 @@
       </c>
       <c r="X95" t="s">
         <v>479</v>
+      </c>
+      <c r="AA95" t="s">
+        <v>669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>